<commit_message>
modified:   main.ipynb 	modified:   "\347\233\243\350\200\203\346\231\202\351\226\223\350\241\250.xlsx"
</commit_message>
<xml_diff>
--- a/監考時間表.xlsx
+++ b/監考時間表.xlsx
@@ -5268,7 +5268,7 @@
         <v>455</v>
       </c>
       <c r="G2" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C2</f>
+        <f>G168*C2</f>
         <v/>
       </c>
       <c r="H2" s="13">
@@ -5745,7 +5745,7 @@
         <v>485</v>
       </c>
       <c r="G7" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C7</f>
+        <f>G168*C7</f>
         <v/>
       </c>
       <c r="H7" s="13">
@@ -6092,7 +6092,7 @@
         <v>470</v>
       </c>
       <c r="G11" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C11</f>
+        <f>G168*C11</f>
         <v/>
       </c>
       <c r="H11" s="13">
@@ -6373,7 +6373,7 @@
         <v>470</v>
       </c>
       <c r="G14" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C14</f>
+        <f>G168*C14</f>
         <v/>
       </c>
       <c r="H14" s="13">
@@ -6585,7 +6585,7 @@
         <v>475</v>
       </c>
       <c r="G16" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C16</f>
+        <f>G168*C16</f>
         <v/>
       </c>
       <c r="H16" s="13">
@@ -6782,7 +6782,7 @@
         <v>475</v>
       </c>
       <c r="G18" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C18</f>
+        <f>G168*C18</f>
         <v/>
       </c>
       <c r="H18" s="13">
@@ -6976,7 +6976,7 @@
         <v>470</v>
       </c>
       <c r="G20" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C20</f>
+        <f>G168*C20</f>
         <v/>
       </c>
       <c r="H20" s="13">
@@ -7386,7 +7386,7 @@
         <v>475</v>
       </c>
       <c r="G24" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C24</f>
+        <f>G168*C24</f>
         <v/>
       </c>
       <c r="H24" s="13">
@@ -7584,7 +7584,7 @@
         <v>135</v>
       </c>
       <c r="G26" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C26</f>
+        <f>G168*C26</f>
         <v/>
       </c>
       <c r="H26" s="11">
@@ -7665,7 +7665,7 @@
         <v>480</v>
       </c>
       <c r="G27" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C27</f>
+        <f>G168*C27</f>
         <v/>
       </c>
       <c r="H27" s="13">
@@ -7924,7 +7924,7 @@
         <v>470</v>
       </c>
       <c r="G29" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C29</f>
+        <f>G168*C29</f>
         <v/>
       </c>
       <c r="H29" s="13">
@@ -8334,7 +8334,7 @@
         <v>485</v>
       </c>
       <c r="G33" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C33</f>
+        <f>G168*C33</f>
         <v/>
       </c>
       <c r="H33" s="13">
@@ -8682,7 +8682,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C36</f>
+        <f>G168*C36</f>
         <v/>
       </c>
       <c r="H36" s="11">
@@ -8749,7 +8749,7 @@
         <v>470</v>
       </c>
       <c r="G37" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C37</f>
+        <f>G168*C37</f>
         <v/>
       </c>
       <c r="H37" s="13">
@@ -9051,7 +9051,7 @@
         <v>500</v>
       </c>
       <c r="G40" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C40</f>
+        <f>G168*C40</f>
         <v/>
       </c>
       <c r="H40" s="13">
@@ -9352,7 +9352,7 @@
         <v>240</v>
       </c>
       <c r="G43" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C43</f>
+        <f>G168*C43</f>
         <v/>
       </c>
       <c r="H43" s="11">
@@ -9447,7 +9447,7 @@
         <v>490</v>
       </c>
       <c r="G44" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C44</f>
+        <f>G168*C44</f>
         <v/>
       </c>
       <c r="H44" s="13">
@@ -9679,7 +9679,7 @@
         <v>475</v>
       </c>
       <c r="G46" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C46</f>
+        <f>G168*C46</f>
         <v/>
       </c>
       <c r="H46" s="13">
@@ -10104,7 +10104,7 @@
         <v>485</v>
       </c>
       <c r="G50" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C50</f>
+        <f>G168*C50</f>
         <v/>
       </c>
       <c r="H50" s="13">
@@ -10524,7 +10524,7 @@
         <v>480</v>
       </c>
       <c r="G54" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C54</f>
+        <f>G168*C54</f>
         <v/>
       </c>
       <c r="H54" s="13">
@@ -10843,7 +10843,7 @@
         <v>470</v>
       </c>
       <c r="G57" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C57</f>
+        <f>G168*C57</f>
         <v/>
       </c>
       <c r="H57" s="13">
@@ -11061,7 +11061,7 @@
         <v>480</v>
       </c>
       <c r="G59" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C59</f>
+        <f>G168*C59</f>
         <v/>
       </c>
       <c r="H59" s="13">
@@ -11517,7 +11517,7 @@
         <v>470</v>
       </c>
       <c r="G64" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C64</f>
+        <f>G168*C64</f>
         <v/>
       </c>
       <c r="H64" s="13">
@@ -11864,7 +11864,7 @@
         <v>470</v>
       </c>
       <c r="G68" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C68</f>
+        <f>G168*C68</f>
         <v/>
       </c>
       <c r="H68" s="13">
@@ -12105,7 +12105,7 @@
         <v>625</v>
       </c>
       <c r="G70" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C70</f>
+        <f>G168*C70</f>
         <v/>
       </c>
       <c r="H70" s="13">
@@ -12653,7 +12653,7 @@
         <v>470</v>
       </c>
       <c r="G76" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C76</f>
+        <f>G168*C76</f>
         <v/>
       </c>
       <c r="H76" s="11">
@@ -12805,7 +12805,7 @@
         <v>475</v>
       </c>
       <c r="G77" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C77</f>
+        <f>G168*C77</f>
         <v/>
       </c>
       <c r="H77" s="13">
@@ -12999,7 +12999,7 @@
         <v>470</v>
       </c>
       <c r="G79" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C79</f>
+        <f>G168*C79</f>
         <v/>
       </c>
       <c r="H79" s="13">
@@ -13286,7 +13286,7 @@
         <v>470</v>
       </c>
       <c r="G82" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C82</f>
+        <f>G168*C82</f>
         <v/>
       </c>
       <c r="H82" s="13">
@@ -13569,7 +13569,7 @@
         <v>470</v>
       </c>
       <c r="G85" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C85</f>
+        <f>G168*C85</f>
         <v/>
       </c>
       <c r="H85" s="13">
@@ -14020,7 +14020,7 @@
         <v>485</v>
       </c>
       <c r="G90" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C90</f>
+        <f>G168*C90</f>
         <v/>
       </c>
       <c r="H90" s="13">
@@ -14444,7 +14444,7 @@
         <v>480</v>
       </c>
       <c r="G94" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C94</f>
+        <f>G168*C94</f>
         <v/>
       </c>
       <c r="H94" s="13">
@@ -14638,7 +14638,7 @@
         <v>485</v>
       </c>
       <c r="G96" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C96</f>
+        <f>G168*C96</f>
         <v/>
       </c>
       <c r="H96" s="13">
@@ -14975,7 +14975,7 @@
         <v>255</v>
       </c>
       <c r="G99" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C99</f>
+        <f>G168*C99</f>
         <v/>
       </c>
       <c r="H99" s="13">
@@ -15254,7 +15254,7 @@
         <v>470</v>
       </c>
       <c r="G102" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C102</f>
+        <f>G168*C102</f>
         <v/>
       </c>
       <c r="H102" s="13">
@@ -15555,7 +15555,7 @@
         <v>470</v>
       </c>
       <c r="G105" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C105</f>
+        <f>G168*C105</f>
         <v/>
       </c>
       <c r="H105" s="13">
@@ -15839,7 +15839,7 @@
         <v>480</v>
       </c>
       <c r="G108" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C108</f>
+        <f>G168*C108</f>
         <v/>
       </c>
       <c r="H108" s="13">
@@ -16037,7 +16037,7 @@
         <v>495</v>
       </c>
       <c r="G110" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C110</f>
+        <f>G168*C110</f>
         <v/>
       </c>
       <c r="H110" s="13">
@@ -16244,7 +16244,7 @@
         <v>495</v>
       </c>
       <c r="G112" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C112</f>
+        <f>G168*C112</f>
         <v/>
       </c>
       <c r="H112" s="13">
@@ -16452,7 +16452,7 @@
         <v>495</v>
       </c>
       <c r="G114" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C114</f>
+        <f>G168*C114</f>
         <v/>
       </c>
       <c r="H114" s="13">
@@ -16665,7 +16665,7 @@
         <v>465</v>
       </c>
       <c r="G116" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C116</f>
+        <f>G168*C116</f>
         <v/>
       </c>
       <c r="H116" s="13">
@@ -16861,7 +16861,7 @@
         <v>470</v>
       </c>
       <c r="G118" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C118</f>
+        <f>G168*C118</f>
         <v/>
       </c>
       <c r="H118" s="13">
@@ -17074,7 +17074,7 @@
         <v>0</v>
       </c>
       <c r="G120" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C120</f>
+        <f>G168*C120</f>
         <v/>
       </c>
       <c r="H120" s="11">
@@ -17137,7 +17137,7 @@
         <v>135</v>
       </c>
       <c r="G121" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C121</f>
+        <f>G168*C121</f>
         <v/>
       </c>
       <c r="H121" s="11">
@@ -17214,7 +17214,7 @@
         <v>135</v>
       </c>
       <c r="G122" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C122</f>
+        <f>G168*C122</f>
         <v/>
       </c>
       <c r="H122" s="11">
@@ -17295,7 +17295,7 @@
         <v>465</v>
       </c>
       <c r="G123" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C123</f>
+        <f>G168*C123</f>
         <v/>
       </c>
       <c r="H123" s="13">
@@ -17496,7 +17496,7 @@
         <v>475</v>
       </c>
       <c r="G125" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C125</f>
+        <f>G168*C125</f>
         <v/>
       </c>
       <c r="H125" s="13">
@@ -17976,7 +17976,7 @@
         <v>465</v>
       </c>
       <c r="G130" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C130</f>
+        <f>G168*C130</f>
         <v/>
       </c>
       <c r="H130" s="13">
@@ -18173,7 +18173,7 @@
         <v>0</v>
       </c>
       <c r="G132" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C132</f>
+        <f>G168*C132</f>
         <v/>
       </c>
       <c r="H132" s="11">
@@ -18240,7 +18240,7 @@
         <v>485</v>
       </c>
       <c r="G133" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C133</f>
+        <f>G168*C133</f>
         <v/>
       </c>
       <c r="H133" s="13">
@@ -18471,7 +18471,7 @@
         <v>470</v>
       </c>
       <c r="G135" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C135</f>
+        <f>G168*C135</f>
         <v/>
       </c>
       <c r="H135" s="13">
@@ -18775,7 +18775,7 @@
         <v>465</v>
       </c>
       <c r="G138" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C138</f>
+        <f>G168*C138</f>
         <v/>
       </c>
       <c r="H138" s="13">
@@ -19127,7 +19127,7 @@
         <v>470</v>
       </c>
       <c r="G142" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C142</f>
+        <f>G168*C142</f>
         <v/>
       </c>
       <c r="H142" s="13">
@@ -19454,7 +19454,7 @@
         <v>495</v>
       </c>
       <c r="G145" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C145</f>
+        <f>G168*C145</f>
         <v/>
       </c>
       <c r="H145" s="13">
@@ -19858,7 +19858,7 @@
         <v>465</v>
       </c>
       <c r="G149" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C149</f>
+        <f>G168*C149</f>
         <v/>
       </c>
       <c r="H149" s="13">
@@ -20059,7 +20059,7 @@
         <v>490</v>
       </c>
       <c r="G151" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C151</f>
+        <f>G168*C151</f>
         <v/>
       </c>
       <c r="H151" s="13">
@@ -20336,7 +20336,7 @@
         <v>480</v>
       </c>
       <c r="G154" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C154</f>
+        <f>G168*C154</f>
         <v/>
       </c>
       <c r="H154" s="13">
@@ -20744,7 +20744,7 @@
         <v>470</v>
       </c>
       <c r="G158" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C158</f>
+        <f>G168*C158</f>
         <v/>
       </c>
       <c r="H158" s="13">
@@ -21041,7 +21041,7 @@
         <v>255</v>
       </c>
       <c r="G161" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C161</f>
+        <f>G168*C161</f>
         <v/>
       </c>
       <c r="H161" s="11">
@@ -21147,7 +21147,7 @@
         <v>255</v>
       </c>
       <c r="G162" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C162</f>
+        <f>G168*C162</f>
         <v/>
       </c>
       <c r="H162" s="11">
@@ -21254,7 +21254,7 @@
         <v>315</v>
       </c>
       <c r="G163" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C163</f>
+        <f>G168*C163</f>
         <v/>
       </c>
       <c r="H163" s="11">
@@ -21360,7 +21360,7 @@
         <v>385</v>
       </c>
       <c r="G164" s="12">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C164</f>
+        <f>G168*C164</f>
         <v/>
       </c>
       <c r="H164" s="13">
@@ -21525,7 +21525,7 @@
         <v>370</v>
       </c>
       <c r="G166" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C166</f>
+        <f>G168*C166</f>
         <v/>
       </c>
       <c r="H166" s="11">
@@ -21646,7 +21646,7 @@
         <v>345</v>
       </c>
       <c r="G167" s="10">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C167</f>
+        <f>G168*C167</f>
         <v/>
       </c>
       <c r="H167" s="11">
@@ -21734,7 +21734,7 @@
     </row>
     <row r="168">
       <c r="G168">
-        <f>((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167))*C168</f>
+        <f>ROUND((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167),0)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
modified:   __pycache__/function_set.cpython-311.pyc 	modified:   function_set.py 	modified:   main.ipynb 	modified:   main.py 	modified:   "\347\233\243\350\200\203\346\231\202\351\226\223\350\241\250.xlsx"
</commit_message>
<xml_diff>
--- a/監考時間表.xlsx
+++ b/監考時間表.xlsx
@@ -5268,7 +5268,7 @@
         <v>455</v>
       </c>
       <c r="G2" s="12">
-        <f>G168*C2</f>
+        <f>ROUND(G168*C2, 0)</f>
         <v/>
       </c>
       <c r="H2" s="13">
@@ -5745,7 +5745,7 @@
         <v>485</v>
       </c>
       <c r="G7" s="12">
-        <f>G168*C7</f>
+        <f>ROUND(G168*C7, 0)</f>
         <v/>
       </c>
       <c r="H7" s="13">
@@ -6092,7 +6092,7 @@
         <v>470</v>
       </c>
       <c r="G11" s="12">
-        <f>G168*C11</f>
+        <f>ROUND(G168*C11, 0)</f>
         <v/>
       </c>
       <c r="H11" s="13">
@@ -6373,7 +6373,7 @@
         <v>470</v>
       </c>
       <c r="G14" s="12">
-        <f>G168*C14</f>
+        <f>ROUND(G168*C14, 0)</f>
         <v/>
       </c>
       <c r="H14" s="13">
@@ -6585,7 +6585,7 @@
         <v>475</v>
       </c>
       <c r="G16" s="12">
-        <f>G168*C16</f>
+        <f>ROUND(G168*C16, 0)</f>
         <v/>
       </c>
       <c r="H16" s="13">
@@ -6782,7 +6782,7 @@
         <v>475</v>
       </c>
       <c r="G18" s="12">
-        <f>G168*C18</f>
+        <f>ROUND(G168*C18, 0)</f>
         <v/>
       </c>
       <c r="H18" s="13">
@@ -6976,7 +6976,7 @@
         <v>470</v>
       </c>
       <c r="G20" s="12">
-        <f>G168*C20</f>
+        <f>ROUND(G168*C20, 0)</f>
         <v/>
       </c>
       <c r="H20" s="13">
@@ -7386,7 +7386,7 @@
         <v>475</v>
       </c>
       <c r="G24" s="12">
-        <f>G168*C24</f>
+        <f>ROUND(G168*C24, 0)</f>
         <v/>
       </c>
       <c r="H24" s="13">
@@ -7584,7 +7584,7 @@
         <v>135</v>
       </c>
       <c r="G26" s="10">
-        <f>G168*C26</f>
+        <f>ROUND(G168*C26, 0)</f>
         <v/>
       </c>
       <c r="H26" s="11">
@@ -7665,7 +7665,7 @@
         <v>480</v>
       </c>
       <c r="G27" s="12">
-        <f>G168*C27</f>
+        <f>ROUND(G168*C27, 0)</f>
         <v/>
       </c>
       <c r="H27" s="13">
@@ -7924,7 +7924,7 @@
         <v>470</v>
       </c>
       <c r="G29" s="12">
-        <f>G168*C29</f>
+        <f>ROUND(G168*C29, 0)</f>
         <v/>
       </c>
       <c r="H29" s="13">
@@ -8334,7 +8334,7 @@
         <v>485</v>
       </c>
       <c r="G33" s="12">
-        <f>G168*C33</f>
+        <f>ROUND(G168*C33, 0)</f>
         <v/>
       </c>
       <c r="H33" s="13">
@@ -8682,7 +8682,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="10">
-        <f>G168*C36</f>
+        <f>ROUND(G168*C36, 0)</f>
         <v/>
       </c>
       <c r="H36" s="11">
@@ -8749,7 +8749,7 @@
         <v>470</v>
       </c>
       <c r="G37" s="12">
-        <f>G168*C37</f>
+        <f>ROUND(G168*C37, 0)</f>
         <v/>
       </c>
       <c r="H37" s="13">
@@ -9051,7 +9051,7 @@
         <v>500</v>
       </c>
       <c r="G40" s="12">
-        <f>G168*C40</f>
+        <f>ROUND(G168*C40, 0)</f>
         <v/>
       </c>
       <c r="H40" s="13">
@@ -9352,7 +9352,7 @@
         <v>240</v>
       </c>
       <c r="G43" s="10">
-        <f>G168*C43</f>
+        <f>ROUND(G168*C43, 0)</f>
         <v/>
       </c>
       <c r="H43" s="11">
@@ -9447,7 +9447,7 @@
         <v>490</v>
       </c>
       <c r="G44" s="12">
-        <f>G168*C44</f>
+        <f>ROUND(G168*C44, 0)</f>
         <v/>
       </c>
       <c r="H44" s="13">
@@ -9679,7 +9679,7 @@
         <v>475</v>
       </c>
       <c r="G46" s="12">
-        <f>G168*C46</f>
+        <f>ROUND(G168*C46, 0)</f>
         <v/>
       </c>
       <c r="H46" s="13">
@@ -10104,7 +10104,7 @@
         <v>485</v>
       </c>
       <c r="G50" s="12">
-        <f>G168*C50</f>
+        <f>ROUND(G168*C50, 0)</f>
         <v/>
       </c>
       <c r="H50" s="13">
@@ -10524,7 +10524,7 @@
         <v>480</v>
       </c>
       <c r="G54" s="12">
-        <f>G168*C54</f>
+        <f>ROUND(G168*C54, 0)</f>
         <v/>
       </c>
       <c r="H54" s="13">
@@ -10843,7 +10843,7 @@
         <v>470</v>
       </c>
       <c r="G57" s="12">
-        <f>G168*C57</f>
+        <f>ROUND(G168*C57, 0)</f>
         <v/>
       </c>
       <c r="H57" s="13">
@@ -11061,7 +11061,7 @@
         <v>480</v>
       </c>
       <c r="G59" s="12">
-        <f>G168*C59</f>
+        <f>ROUND(G168*C59, 0)</f>
         <v/>
       </c>
       <c r="H59" s="13">
@@ -11517,7 +11517,7 @@
         <v>470</v>
       </c>
       <c r="G64" s="12">
-        <f>G168*C64</f>
+        <f>ROUND(G168*C64, 0)</f>
         <v/>
       </c>
       <c r="H64" s="13">
@@ -11864,7 +11864,7 @@
         <v>470</v>
       </c>
       <c r="G68" s="12">
-        <f>G168*C68</f>
+        <f>ROUND(G168*C68, 0)</f>
         <v/>
       </c>
       <c r="H68" s="13">
@@ -12105,7 +12105,7 @@
         <v>625</v>
       </c>
       <c r="G70" s="12">
-        <f>G168*C70</f>
+        <f>ROUND(G168*C70, 0)</f>
         <v/>
       </c>
       <c r="H70" s="13">
@@ -12653,7 +12653,7 @@
         <v>470</v>
       </c>
       <c r="G76" s="10">
-        <f>G168*C76</f>
+        <f>ROUND(G168*C76, 0)</f>
         <v/>
       </c>
       <c r="H76" s="11">
@@ -12805,7 +12805,7 @@
         <v>475</v>
       </c>
       <c r="G77" s="12">
-        <f>G168*C77</f>
+        <f>ROUND(G168*C77, 0)</f>
         <v/>
       </c>
       <c r="H77" s="13">
@@ -12999,7 +12999,7 @@
         <v>470</v>
       </c>
       <c r="G79" s="12">
-        <f>G168*C79</f>
+        <f>ROUND(G168*C79, 0)</f>
         <v/>
       </c>
       <c r="H79" s="13">
@@ -13286,7 +13286,7 @@
         <v>470</v>
       </c>
       <c r="G82" s="12">
-        <f>G168*C82</f>
+        <f>ROUND(G168*C82, 0)</f>
         <v/>
       </c>
       <c r="H82" s="13">
@@ -13569,7 +13569,7 @@
         <v>470</v>
       </c>
       <c r="G85" s="12">
-        <f>G168*C85</f>
+        <f>ROUND(G168*C85, 0)</f>
         <v/>
       </c>
       <c r="H85" s="13">
@@ -14020,7 +14020,7 @@
         <v>485</v>
       </c>
       <c r="G90" s="12">
-        <f>G168*C90</f>
+        <f>ROUND(G168*C90, 0)</f>
         <v/>
       </c>
       <c r="H90" s="13">
@@ -14444,7 +14444,7 @@
         <v>480</v>
       </c>
       <c r="G94" s="12">
-        <f>G168*C94</f>
+        <f>ROUND(G168*C94, 0)</f>
         <v/>
       </c>
       <c r="H94" s="13">
@@ -14638,7 +14638,7 @@
         <v>485</v>
       </c>
       <c r="G96" s="12">
-        <f>G168*C96</f>
+        <f>ROUND(G168*C96, 0)</f>
         <v/>
       </c>
       <c r="H96" s="13">
@@ -14975,7 +14975,7 @@
         <v>255</v>
       </c>
       <c r="G99" s="12">
-        <f>G168*C99</f>
+        <f>ROUND(G168*C99, 0)</f>
         <v/>
       </c>
       <c r="H99" s="13">
@@ -15254,7 +15254,7 @@
         <v>470</v>
       </c>
       <c r="G102" s="12">
-        <f>G168*C102</f>
+        <f>ROUND(G168*C102, 0)</f>
         <v/>
       </c>
       <c r="H102" s="13">
@@ -15555,7 +15555,7 @@
         <v>470</v>
       </c>
       <c r="G105" s="12">
-        <f>G168*C105</f>
+        <f>ROUND(G168*C105, 0)</f>
         <v/>
       </c>
       <c r="H105" s="13">
@@ -15839,7 +15839,7 @@
         <v>480</v>
       </c>
       <c r="G108" s="12">
-        <f>G168*C108</f>
+        <f>ROUND(G168*C108, 0)</f>
         <v/>
       </c>
       <c r="H108" s="13">
@@ -16037,7 +16037,7 @@
         <v>495</v>
       </c>
       <c r="G110" s="12">
-        <f>G168*C110</f>
+        <f>ROUND(G168*C110, 0)</f>
         <v/>
       </c>
       <c r="H110" s="13">
@@ -16244,7 +16244,7 @@
         <v>495</v>
       </c>
       <c r="G112" s="12">
-        <f>G168*C112</f>
+        <f>ROUND(G168*C112, 0)</f>
         <v/>
       </c>
       <c r="H112" s="13">
@@ -16452,7 +16452,7 @@
         <v>495</v>
       </c>
       <c r="G114" s="12">
-        <f>G168*C114</f>
+        <f>ROUND(G168*C114, 0)</f>
         <v/>
       </c>
       <c r="H114" s="13">
@@ -16665,7 +16665,7 @@
         <v>465</v>
       </c>
       <c r="G116" s="12">
-        <f>G168*C116</f>
+        <f>ROUND(G168*C116, 0)</f>
         <v/>
       </c>
       <c r="H116" s="13">
@@ -16861,7 +16861,7 @@
         <v>470</v>
       </c>
       <c r="G118" s="12">
-        <f>G168*C118</f>
+        <f>ROUND(G168*C118, 0)</f>
         <v/>
       </c>
       <c r="H118" s="13">
@@ -17074,7 +17074,7 @@
         <v>0</v>
       </c>
       <c r="G120" s="10">
-        <f>G168*C120</f>
+        <f>ROUND(G168*C120, 0)</f>
         <v/>
       </c>
       <c r="H120" s="11">
@@ -17137,7 +17137,7 @@
         <v>135</v>
       </c>
       <c r="G121" s="10">
-        <f>G168*C121</f>
+        <f>ROUND(G168*C121, 0)</f>
         <v/>
       </c>
       <c r="H121" s="11">
@@ -17214,7 +17214,7 @@
         <v>135</v>
       </c>
       <c r="G122" s="10">
-        <f>G168*C122</f>
+        <f>ROUND(G168*C122, 0)</f>
         <v/>
       </c>
       <c r="H122" s="11">
@@ -17295,7 +17295,7 @@
         <v>465</v>
       </c>
       <c r="G123" s="12">
-        <f>G168*C123</f>
+        <f>ROUND(G168*C123, 0)</f>
         <v/>
       </c>
       <c r="H123" s="13">
@@ -17496,7 +17496,7 @@
         <v>475</v>
       </c>
       <c r="G125" s="12">
-        <f>G168*C125</f>
+        <f>ROUND(G168*C125, 0)</f>
         <v/>
       </c>
       <c r="H125" s="13">
@@ -17976,7 +17976,7 @@
         <v>465</v>
       </c>
       <c r="G130" s="12">
-        <f>G168*C130</f>
+        <f>ROUND(G168*C130, 0)</f>
         <v/>
       </c>
       <c r="H130" s="13">
@@ -18173,7 +18173,7 @@
         <v>0</v>
       </c>
       <c r="G132" s="10">
-        <f>G168*C132</f>
+        <f>ROUND(G168*C132, 0)</f>
         <v/>
       </c>
       <c r="H132" s="11">
@@ -18240,7 +18240,7 @@
         <v>485</v>
       </c>
       <c r="G133" s="12">
-        <f>G168*C133</f>
+        <f>ROUND(G168*C133, 0)</f>
         <v/>
       </c>
       <c r="H133" s="13">
@@ -18471,7 +18471,7 @@
         <v>470</v>
       </c>
       <c r="G135" s="12">
-        <f>G168*C135</f>
+        <f>ROUND(G168*C135, 0)</f>
         <v/>
       </c>
       <c r="H135" s="13">
@@ -18775,7 +18775,7 @@
         <v>465</v>
       </c>
       <c r="G138" s="12">
-        <f>G168*C138</f>
+        <f>ROUND(G168*C138, 0)</f>
         <v/>
       </c>
       <c r="H138" s="13">
@@ -19127,7 +19127,7 @@
         <v>470</v>
       </c>
       <c r="G142" s="12">
-        <f>G168*C142</f>
+        <f>ROUND(G168*C142, 0)</f>
         <v/>
       </c>
       <c r="H142" s="13">
@@ -19454,7 +19454,7 @@
         <v>495</v>
       </c>
       <c r="G145" s="12">
-        <f>G168*C145</f>
+        <f>ROUND(G168*C145, 0)</f>
         <v/>
       </c>
       <c r="H145" s="13">
@@ -19858,7 +19858,7 @@
         <v>465</v>
       </c>
       <c r="G149" s="12">
-        <f>G168*C149</f>
+        <f>ROUND(G168*C149, 0)</f>
         <v/>
       </c>
       <c r="H149" s="13">
@@ -20059,7 +20059,7 @@
         <v>490</v>
       </c>
       <c r="G151" s="12">
-        <f>G168*C151</f>
+        <f>ROUND(G168*C151, 0)</f>
         <v/>
       </c>
       <c r="H151" s="13">
@@ -20336,7 +20336,7 @@
         <v>480</v>
       </c>
       <c r="G154" s="12">
-        <f>G168*C154</f>
+        <f>ROUND(G168*C154, 0)</f>
         <v/>
       </c>
       <c r="H154" s="13">
@@ -20744,7 +20744,7 @@
         <v>470</v>
       </c>
       <c r="G158" s="12">
-        <f>G168*C158</f>
+        <f>ROUND(G168*C158, 0)</f>
         <v/>
       </c>
       <c r="H158" s="13">
@@ -21041,7 +21041,7 @@
         <v>255</v>
       </c>
       <c r="G161" s="10">
-        <f>G168*C161</f>
+        <f>ROUND(G168*C161, 0)</f>
         <v/>
       </c>
       <c r="H161" s="11">
@@ -21147,7 +21147,7 @@
         <v>255</v>
       </c>
       <c r="G162" s="10">
-        <f>G168*C162</f>
+        <f>ROUND(G168*C162, 0)</f>
         <v/>
       </c>
       <c r="H162" s="11">
@@ -21254,7 +21254,7 @@
         <v>315</v>
       </c>
       <c r="G163" s="10">
-        <f>G168*C163</f>
+        <f>ROUND(G168*C163, 0)</f>
         <v/>
       </c>
       <c r="H163" s="11">
@@ -21360,7 +21360,7 @@
         <v>385</v>
       </c>
       <c r="G164" s="12">
-        <f>G168*C164</f>
+        <f>ROUND(G168*C164, 0)</f>
         <v/>
       </c>
       <c r="H164" s="13">
@@ -21525,7 +21525,7 @@
         <v>370</v>
       </c>
       <c r="G166" s="10">
-        <f>G168*C166</f>
+        <f>ROUND(G168*C166, 0)</f>
         <v/>
       </c>
       <c r="H166" s="11">
@@ -21646,7 +21646,7 @@
         <v>345</v>
       </c>
       <c r="G167" s="10">
-        <f>G168*C167</f>
+        <f>ROUND(G168*C167, 0)</f>
         <v/>
       </c>
       <c r="H167" s="11">
@@ -21733,8 +21733,24 @@
       </c>
     </row>
     <row r="168">
+      <c r="C168">
+        <f t="array" ref="C168">SUM(C2:C167)</f>
+        <v/>
+      </c>
+      <c r="D168">
+        <f t="array" ref="D168">SUM(D2:D167)</f>
+        <v/>
+      </c>
+      <c r="E168">
+        <f t="array" ref="E168">SUM(E2:E167)</f>
+        <v/>
+      </c>
+      <c r="F168">
+        <f t="array" ref="F168">SUM(F2:F167)</f>
+        <v/>
+      </c>
       <c r="G168">
-        <f>ROUND((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167),0)</f>
+        <f t="array" ref="G168">ROUND((SUM($D$2:$D$167*$C$2:$C$167)-F161-F162-F163-F164+SUM($E$2:$E$167))/SUM($C$2:$C$167),0)</f>
         <v/>
       </c>
     </row>

</xml_diff>